<commit_message>
nuevo formato de excel
</commit_message>
<xml_diff>
--- a/formato evidencias de python shop.xlsx
+++ b/formato evidencias de python shop.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="45">
   <si>
     <t xml:space="preserve">Participantes </t>
   </si>
@@ -157,6 +157,9 @@
   </si>
   <si>
     <t>Hanna maria buelvas maya</t>
+  </si>
+  <si>
+    <t>Edison Bedoya Amaya</t>
   </si>
 </sst>
 </file>
@@ -367,112 +370,103 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -787,7 +781,7 @@
   <dimension ref="A1:I55"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A33" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C48" sqref="C48:E48"/>
+      <selection activeCell="C46" sqref="C46:E46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -796,665 +790,678 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="19"/>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
+      <c r="A2" s="15"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="8"/>
-      <c r="C3" s="20" t="s">
+      <c r="B3" s="16"/>
+      <c r="C3" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="20" t="s">
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="20"/>
-      <c r="H3" s="20"/>
-      <c r="I3" s="20"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="8"/>
-      <c r="B4" s="8"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="20"/>
-      <c r="I4" s="20"/>
+      <c r="A4" s="16"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="19"/>
+      <c r="H4" s="19"/>
+      <c r="I4" s="19"/>
     </row>
     <row r="5" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="8"/>
-      <c r="C5" s="7" t="s">
+      <c r="B5" s="16"/>
+      <c r="C5" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="7"/>
+      <c r="D5" s="17"/>
       <c r="E5" s="18"/>
-      <c r="F5" s="6" t="s">
+      <c r="F5" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
+      <c r="G5" s="21"/>
+      <c r="H5" s="21"/>
+      <c r="I5" s="21"/>
     </row>
     <row r="6" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="8"/>
-      <c r="B6" s="8"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
+      <c r="A6" s="16"/>
+      <c r="B6" s="16"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="17"/>
       <c r="E6" s="18"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
+      <c r="F6" s="21"/>
+      <c r="G6" s="21"/>
+      <c r="H6" s="21"/>
+      <c r="I6" s="21"/>
     </row>
     <row r="7" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="8"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="7" t="s">
+      <c r="A7" s="16"/>
+      <c r="B7" s="16"/>
+      <c r="C7" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="21"/>
+      <c r="G7" s="21"/>
+      <c r="H7" s="21"/>
+      <c r="I7" s="21"/>
     </row>
     <row r="8" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="8"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
+      <c r="A8" s="16"/>
+      <c r="B8" s="16"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="17"/>
       <c r="E8" s="18"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
+      <c r="F8" s="21"/>
+      <c r="G8" s="21"/>
+      <c r="H8" s="21"/>
+      <c r="I8" s="21"/>
     </row>
     <row r="9" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="8"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="12" t="s">
+      <c r="A9" s="16"/>
+      <c r="B9" s="16"/>
+      <c r="C9" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="13"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="11" t="s">
+      <c r="D9" s="24"/>
+      <c r="E9" s="25"/>
+      <c r="F9" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="G9" s="11"/>
-      <c r="H9" s="11"/>
-      <c r="I9" s="11"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="22"/>
+      <c r="I9" s="22"/>
     </row>
     <row r="10" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="8"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="15"/>
-      <c r="D10" s="16"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="11"/>
-      <c r="I10" s="11"/>
+      <c r="A10" s="16"/>
+      <c r="B10" s="16"/>
+      <c r="C10" s="26"/>
+      <c r="D10" s="27"/>
+      <c r="E10" s="28"/>
+      <c r="F10" s="22"/>
+      <c r="G10" s="22"/>
+      <c r="H10" s="22"/>
+      <c r="I10" s="22"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="8"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="7" t="s">
+      <c r="A11" s="16"/>
+      <c r="B11" s="16"/>
+      <c r="C11" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="11"/>
-      <c r="H11" s="11"/>
-      <c r="I11" s="11"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="22"/>
+      <c r="G11" s="22"/>
+      <c r="H11" s="22"/>
+      <c r="I11" s="22"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="8"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
+      <c r="A12" s="16"/>
+      <c r="B12" s="16"/>
+      <c r="C12" s="17"/>
+      <c r="D12" s="17"/>
       <c r="E12" s="18"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="11"/>
-      <c r="H12" s="11"/>
-      <c r="I12" s="11"/>
+      <c r="F12" s="22"/>
+      <c r="G12" s="22"/>
+      <c r="H12" s="22"/>
+      <c r="I12" s="22"/>
     </row>
     <row r="13" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="3"/>
-      <c r="C13" s="6" t="s">
+      <c r="B13" s="1"/>
+      <c r="C13" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6" t="s">
+      <c r="D13" s="21"/>
+      <c r="E13" s="21"/>
+      <c r="F13" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="6"/>
+      <c r="G13" s="21"/>
+      <c r="H13" s="21"/>
+      <c r="I13" s="21"/>
     </row>
     <row r="14" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="4"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="6" t="s">
+      <c r="A14" s="30"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="6"/>
+      <c r="D14" s="21"/>
+      <c r="E14" s="21"/>
+      <c r="F14" s="21"/>
+      <c r="G14" s="21"/>
+      <c r="H14" s="21"/>
+      <c r="I14" s="21"/>
     </row>
     <row r="15" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="4"/>
-      <c r="B15" s="5"/>
-      <c r="C15" s="6" t="s">
+      <c r="A15" s="30"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="6"/>
-      <c r="H15" s="6"/>
-      <c r="I15" s="6"/>
+      <c r="D15" s="21"/>
+      <c r="E15" s="21"/>
+      <c r="F15" s="21"/>
+      <c r="G15" s="21"/>
+      <c r="H15" s="21"/>
+      <c r="I15" s="21"/>
     </row>
     <row r="16" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="4"/>
-      <c r="B16" s="5"/>
-      <c r="C16" s="6" t="s">
+      <c r="A16" s="30"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
-      <c r="I16" s="6"/>
+      <c r="D16" s="21"/>
+      <c r="E16" s="21"/>
+      <c r="F16" s="21"/>
+      <c r="G16" s="21"/>
+      <c r="H16" s="21"/>
+      <c r="I16" s="21"/>
     </row>
     <row r="17" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="4"/>
-      <c r="B17" s="5"/>
-      <c r="C17" s="6" t="s">
+      <c r="A17" s="30"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="6" t="s">
+      <c r="D17" s="21"/>
+      <c r="E17" s="21"/>
+      <c r="F17" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="G17" s="6"/>
-      <c r="H17" s="6"/>
-      <c r="I17" s="6"/>
+      <c r="G17" s="21"/>
+      <c r="H17" s="21"/>
+      <c r="I17" s="21"/>
     </row>
     <row r="18" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="4"/>
-      <c r="B18" s="5"/>
-      <c r="C18" s="6" t="s">
+      <c r="A18" s="30"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="6"/>
-      <c r="H18" s="6"/>
-      <c r="I18" s="6"/>
+      <c r="D18" s="21"/>
+      <c r="E18" s="21"/>
+      <c r="F18" s="21"/>
+      <c r="G18" s="21"/>
+      <c r="H18" s="21"/>
+      <c r="I18" s="21"/>
     </row>
     <row r="19" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="4"/>
-      <c r="B19" s="5"/>
-      <c r="C19" s="6" t="s">
+      <c r="A19" s="30"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="6"/>
-      <c r="H19" s="6"/>
-      <c r="I19" s="6"/>
+      <c r="D19" s="21"/>
+      <c r="E19" s="21"/>
+      <c r="F19" s="21"/>
+      <c r="G19" s="21"/>
+      <c r="H19" s="21"/>
+      <c r="I19" s="21"/>
     </row>
     <row r="20" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="4"/>
-      <c r="B20" s="5"/>
-      <c r="C20" s="6" t="s">
+      <c r="A20" s="30"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="6"/>
-      <c r="H20" s="6"/>
-      <c r="I20" s="6"/>
+      <c r="D20" s="21"/>
+      <c r="E20" s="21"/>
+      <c r="F20" s="21"/>
+      <c r="G20" s="21"/>
+      <c r="H20" s="21"/>
+      <c r="I20" s="21"/>
     </row>
     <row r="21" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="4"/>
-      <c r="B21" s="5"/>
-      <c r="C21" s="6" t="s">
+      <c r="A21" s="30"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="D21" s="6"/>
-      <c r="E21" s="10"/>
-      <c r="F21" s="6" t="s">
+      <c r="D21" s="21"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="G21" s="6"/>
-      <c r="H21" s="6"/>
-      <c r="I21" s="6"/>
+      <c r="G21" s="21"/>
+      <c r="H21" s="21"/>
+      <c r="I21" s="21"/>
     </row>
     <row r="22" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="4"/>
-      <c r="B22" s="5"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="10"/>
-      <c r="F22" s="6"/>
-      <c r="G22" s="6"/>
-      <c r="H22" s="6"/>
-      <c r="I22" s="6"/>
+      <c r="A22" s="30"/>
+      <c r="B22" s="2"/>
+      <c r="C22" s="21"/>
+      <c r="D22" s="21"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="21"/>
+      <c r="G22" s="21"/>
+      <c r="H22" s="21"/>
+      <c r="I22" s="21"/>
     </row>
     <row r="23" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="4"/>
-      <c r="B23" s="5"/>
-      <c r="C23" s="6" t="s">
+      <c r="A23" s="30"/>
+      <c r="B23" s="2"/>
+      <c r="C23" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="D23" s="6"/>
-      <c r="E23" s="10"/>
-      <c r="F23" s="6"/>
-      <c r="G23" s="6"/>
-      <c r="H23" s="6"/>
-      <c r="I23" s="6"/>
+      <c r="D23" s="21"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="21"/>
+      <c r="G23" s="21"/>
+      <c r="H23" s="21"/>
+      <c r="I23" s="21"/>
     </row>
     <row r="24" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="4"/>
-      <c r="B24" s="5"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="6"/>
-      <c r="E24" s="10"/>
-      <c r="F24" s="6"/>
-      <c r="G24" s="6"/>
-      <c r="H24" s="6"/>
-      <c r="I24" s="6"/>
+      <c r="A24" s="30"/>
+      <c r="B24" s="2"/>
+      <c r="C24" s="21"/>
+      <c r="D24" s="21"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="21"/>
+      <c r="G24" s="21"/>
+      <c r="H24" s="21"/>
+      <c r="I24" s="21"/>
     </row>
     <row r="25" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="4"/>
-      <c r="B25" s="5"/>
-      <c r="C25" s="1" t="s">
+      <c r="A25" s="30"/>
+      <c r="B25" s="2"/>
+      <c r="C25" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="6"/>
-      <c r="G25" s="6"/>
-      <c r="H25" s="6"/>
-      <c r="I25" s="6"/>
+      <c r="D25" s="20"/>
+      <c r="E25" s="20"/>
+      <c r="F25" s="21"/>
+      <c r="G25" s="21"/>
+      <c r="H25" s="21"/>
+      <c r="I25" s="21"/>
     </row>
     <row r="26" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="4"/>
-      <c r="B26" s="5"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-      <c r="F26" s="6"/>
-      <c r="G26" s="6"/>
-      <c r="H26" s="6"/>
-      <c r="I26" s="6"/>
+      <c r="A26" s="30"/>
+      <c r="B26" s="2"/>
+      <c r="C26" s="20"/>
+      <c r="D26" s="20"/>
+      <c r="E26" s="20"/>
+      <c r="F26" s="21"/>
+      <c r="G26" s="21"/>
+      <c r="H26" s="21"/>
+      <c r="I26" s="21"/>
     </row>
     <row r="27" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="8" t="s">
+      <c r="A27" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="B27" s="8"/>
-      <c r="C27" s="1" t="s">
+      <c r="B27" s="16"/>
+      <c r="C27" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-      <c r="F27" s="6" t="s">
+      <c r="D27" s="20"/>
+      <c r="E27" s="20"/>
+      <c r="F27" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="G27" s="6"/>
-      <c r="H27" s="6"/>
-      <c r="I27" s="6"/>
+      <c r="G27" s="21"/>
+      <c r="H27" s="21"/>
+      <c r="I27" s="21"/>
     </row>
     <row r="28" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="8"/>
-      <c r="B28" s="8"/>
-      <c r="C28" s="1" t="s">
+      <c r="A28" s="16"/>
+      <c r="B28" s="16"/>
+      <c r="C28" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-      <c r="F28" s="6"/>
-      <c r="G28" s="6"/>
-      <c r="H28" s="6"/>
-      <c r="I28" s="6"/>
+      <c r="D28" s="20"/>
+      <c r="E28" s="20"/>
+      <c r="F28" s="21"/>
+      <c r="G28" s="21"/>
+      <c r="H28" s="21"/>
+      <c r="I28" s="21"/>
     </row>
     <row r="29" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="8"/>
-      <c r="B29" s="8"/>
-      <c r="C29" s="1" t="s">
+      <c r="A29" s="16"/>
+      <c r="B29" s="16"/>
+      <c r="C29" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
-      <c r="F29" s="6"/>
-      <c r="G29" s="6"/>
-      <c r="H29" s="6"/>
-      <c r="I29" s="6"/>
+      <c r="D29" s="20"/>
+      <c r="E29" s="20"/>
+      <c r="F29" s="21"/>
+      <c r="G29" s="21"/>
+      <c r="H29" s="21"/>
+      <c r="I29" s="21"/>
     </row>
     <row r="30" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="8"/>
-      <c r="B30" s="8"/>
-      <c r="C30" s="6" t="s">
+      <c r="A30" s="16"/>
+      <c r="B30" s="16"/>
+      <c r="C30" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="D30" s="6"/>
-      <c r="E30" s="10"/>
-      <c r="F30" s="9" t="s">
+      <c r="D30" s="21"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="G30" s="9"/>
-      <c r="H30" s="9"/>
-      <c r="I30" s="9"/>
+      <c r="G30" s="31"/>
+      <c r="H30" s="31"/>
+      <c r="I30" s="31"/>
     </row>
     <row r="31" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="8"/>
-      <c r="B31" s="8"/>
-      <c r="C31" s="6"/>
-      <c r="D31" s="6"/>
-      <c r="E31" s="10"/>
-      <c r="F31" s="9"/>
-      <c r="G31" s="9"/>
-      <c r="H31" s="9"/>
-      <c r="I31" s="9"/>
+      <c r="A31" s="16"/>
+      <c r="B31" s="16"/>
+      <c r="C31" s="21"/>
+      <c r="D31" s="21"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="31"/>
+      <c r="G31" s="31"/>
+      <c r="H31" s="31"/>
+      <c r="I31" s="31"/>
     </row>
     <row r="32" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="8"/>
-      <c r="B32" s="8"/>
-      <c r="C32" s="1" t="s">
+      <c r="A32" s="16"/>
+      <c r="B32" s="16"/>
+      <c r="C32" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
-      <c r="F32" s="9"/>
-      <c r="G32" s="9"/>
-      <c r="H32" s="9"/>
-      <c r="I32" s="9"/>
+      <c r="D32" s="20"/>
+      <c r="E32" s="20"/>
+      <c r="F32" s="31"/>
+      <c r="G32" s="31"/>
+      <c r="H32" s="31"/>
+      <c r="I32" s="31"/>
     </row>
     <row r="33" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="8"/>
-      <c r="B33" s="8"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="1"/>
-      <c r="E33" s="1"/>
-      <c r="F33" s="9"/>
-      <c r="G33" s="9"/>
-      <c r="H33" s="9"/>
-      <c r="I33" s="9"/>
+      <c r="A33" s="16"/>
+      <c r="B33" s="16"/>
+      <c r="C33" s="20"/>
+      <c r="D33" s="20"/>
+      <c r="E33" s="20"/>
+      <c r="F33" s="31"/>
+      <c r="G33" s="31"/>
+      <c r="H33" s="31"/>
+      <c r="I33" s="31"/>
     </row>
     <row r="34" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="8"/>
-      <c r="B34" s="8"/>
-      <c r="C34" s="7" t="s">
+      <c r="A34" s="16"/>
+      <c r="B34" s="16"/>
+      <c r="C34" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="D34" s="7"/>
-      <c r="E34" s="7"/>
-      <c r="F34" s="6" t="s">
+      <c r="D34" s="17"/>
+      <c r="E34" s="17"/>
+      <c r="F34" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="G34" s="6"/>
-      <c r="H34" s="6"/>
-      <c r="I34" s="6"/>
+      <c r="G34" s="21"/>
+      <c r="H34" s="21"/>
+      <c r="I34" s="21"/>
     </row>
     <row r="35" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="8"/>
-      <c r="B35" s="8"/>
-      <c r="C35" s="7"/>
-      <c r="D35" s="7"/>
-      <c r="E35" s="7"/>
-      <c r="F35" s="6"/>
-      <c r="G35" s="6"/>
-      <c r="H35" s="6"/>
-      <c r="I35" s="6"/>
+      <c r="A35" s="16"/>
+      <c r="B35" s="16"/>
+      <c r="C35" s="17"/>
+      <c r="D35" s="17"/>
+      <c r="E35" s="17"/>
+      <c r="F35" s="21"/>
+      <c r="G35" s="21"/>
+      <c r="H35" s="21"/>
+      <c r="I35" s="21"/>
     </row>
     <row r="36" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="8"/>
-      <c r="B36" s="8"/>
-      <c r="C36" s="7"/>
-      <c r="D36" s="7"/>
-      <c r="E36" s="7"/>
-      <c r="F36" s="6"/>
-      <c r="G36" s="6"/>
-      <c r="H36" s="6"/>
-      <c r="I36" s="6"/>
+      <c r="A36" s="16"/>
+      <c r="B36" s="16"/>
+      <c r="C36" s="17"/>
+      <c r="D36" s="17"/>
+      <c r="E36" s="17"/>
+      <c r="F36" s="21"/>
+      <c r="G36" s="21"/>
+      <c r="H36" s="21"/>
+      <c r="I36" s="21"/>
     </row>
     <row r="37" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="8"/>
-      <c r="B37" s="8"/>
-      <c r="C37" s="6" t="s">
+      <c r="A37" s="16"/>
+      <c r="B37" s="16"/>
+      <c r="C37" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="D37" s="6"/>
-      <c r="E37" s="6"/>
-      <c r="F37" s="6" t="s">
+      <c r="D37" s="21"/>
+      <c r="E37" s="21"/>
+      <c r="F37" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="G37" s="6"/>
-      <c r="H37" s="6"/>
-      <c r="I37" s="6"/>
+      <c r="G37" s="21"/>
+      <c r="H37" s="21"/>
+      <c r="I37" s="21"/>
     </row>
     <row r="38" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="8"/>
-      <c r="B38" s="8"/>
-      <c r="C38" s="6"/>
-      <c r="D38" s="6"/>
-      <c r="E38" s="6"/>
-      <c r="F38" s="6"/>
-      <c r="G38" s="6"/>
-      <c r="H38" s="6"/>
-      <c r="I38" s="6"/>
+      <c r="A38" s="16"/>
+      <c r="B38" s="16"/>
+      <c r="C38" s="21"/>
+      <c r="D38" s="21"/>
+      <c r="E38" s="21"/>
+      <c r="F38" s="21"/>
+      <c r="G38" s="21"/>
+      <c r="H38" s="21"/>
+      <c r="I38" s="21"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39" s="8"/>
-      <c r="B39" s="8"/>
-      <c r="C39" s="6"/>
-      <c r="D39" s="6"/>
-      <c r="E39" s="6"/>
-      <c r="F39" s="6"/>
-      <c r="G39" s="6"/>
-      <c r="H39" s="6"/>
-      <c r="I39" s="6"/>
+      <c r="A39" s="16"/>
+      <c r="B39" s="16"/>
+      <c r="C39" s="21"/>
+      <c r="D39" s="21"/>
+      <c r="E39" s="21"/>
+      <c r="F39" s="21"/>
+      <c r="G39" s="21"/>
+      <c r="H39" s="21"/>
+      <c r="I39" s="21"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A40" s="8"/>
-      <c r="B40" s="8"/>
-      <c r="C40" s="6"/>
-      <c r="D40" s="6"/>
-      <c r="E40" s="6"/>
-      <c r="F40" s="6"/>
-      <c r="G40" s="6"/>
-      <c r="H40" s="6"/>
-      <c r="I40" s="6"/>
+      <c r="A40" s="16"/>
+      <c r="B40" s="16"/>
+      <c r="C40" s="21"/>
+      <c r="D40" s="21"/>
+      <c r="E40" s="21"/>
+      <c r="F40" s="21"/>
+      <c r="G40" s="21"/>
+      <c r="H40" s="21"/>
+      <c r="I40" s="21"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A41" s="8"/>
-      <c r="B41" s="8"/>
-      <c r="C41" s="6"/>
-      <c r="D41" s="6"/>
-      <c r="E41" s="6"/>
-      <c r="F41" s="6"/>
-      <c r="G41" s="6"/>
-      <c r="H41" s="6"/>
-      <c r="I41" s="6"/>
+      <c r="A41" s="16"/>
+      <c r="B41" s="16"/>
+      <c r="C41" s="21"/>
+      <c r="D41" s="21"/>
+      <c r="E41" s="21"/>
+      <c r="F41" s="21"/>
+      <c r="G41" s="21"/>
+      <c r="H41" s="21"/>
+      <c r="I41" s="21"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A42" s="8"/>
-      <c r="B42" s="8"/>
-      <c r="C42" s="6"/>
-      <c r="D42" s="6"/>
-      <c r="E42" s="6"/>
-      <c r="F42" s="6"/>
-      <c r="G42" s="6"/>
-      <c r="H42" s="6"/>
-      <c r="I42" s="6"/>
+      <c r="A42" s="16"/>
+      <c r="B42" s="16"/>
+      <c r="C42" s="21"/>
+      <c r="D42" s="21"/>
+      <c r="E42" s="21"/>
+      <c r="F42" s="21"/>
+      <c r="G42" s="21"/>
+      <c r="H42" s="21"/>
+      <c r="I42" s="21"/>
     </row>
     <row r="43" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="32" t="s">
+      <c r="A43" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="B43" s="3"/>
-      <c r="C43" s="23" t="s">
+      <c r="B43" s="16"/>
+      <c r="C43" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="D43" s="24"/>
-      <c r="E43" s="25"/>
-      <c r="F43" s="23" t="s">
+      <c r="D43" s="7"/>
+      <c r="E43" s="8"/>
+      <c r="F43" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="G43" s="24"/>
-      <c r="H43" s="24"/>
-      <c r="I43" s="25"/>
+      <c r="G43" s="7"/>
+      <c r="H43" s="7"/>
+      <c r="I43" s="8"/>
     </row>
     <row r="44" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="33"/>
-      <c r="B44" s="5"/>
-      <c r="C44" s="26"/>
-      <c r="D44" s="27"/>
-      <c r="E44" s="28"/>
-      <c r="F44" s="29"/>
-      <c r="G44" s="30"/>
-      <c r="H44" s="30"/>
-      <c r="I44" s="31"/>
+      <c r="A44" s="16"/>
+      <c r="B44" s="16"/>
+      <c r="C44" s="13"/>
+      <c r="D44" s="13"/>
+      <c r="E44" s="14"/>
+      <c r="F44" s="9"/>
+      <c r="G44" s="10"/>
+      <c r="H44" s="10"/>
+      <c r="I44" s="11"/>
     </row>
     <row r="45" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="33"/>
-      <c r="B45" s="5"/>
-      <c r="C45" s="10" t="s">
+      <c r="A45" s="16"/>
+      <c r="B45" s="16"/>
+      <c r="C45" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="D45" s="21"/>
-      <c r="E45" s="22"/>
-      <c r="F45" s="26"/>
-      <c r="G45" s="27"/>
-      <c r="H45" s="27"/>
-      <c r="I45" s="28"/>
-    </row>
-    <row r="46" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="33"/>
-      <c r="B46" s="5"/>
-      <c r="C46" s="10" t="s">
+      <c r="D45" s="4"/>
+      <c r="E45" s="5"/>
+      <c r="F45" s="12"/>
+      <c r="G45" s="13"/>
+      <c r="H45" s="13"/>
+      <c r="I45" s="14"/>
+    </row>
+    <row r="46" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="16"/>
+      <c r="B46" s="16"/>
+      <c r="C46" s="32" t="s">
+        <v>44</v>
+      </c>
+      <c r="D46" s="32"/>
+      <c r="E46" s="32"/>
+      <c r="F46" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="G46" s="21"/>
+      <c r="H46" s="21"/>
+      <c r="I46" s="21"/>
+    </row>
+    <row r="47" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="16"/>
+      <c r="B47" s="16"/>
+      <c r="C47" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="D46" s="21"/>
-      <c r="E46" s="22"/>
-      <c r="F46" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="G46" s="24"/>
-      <c r="H46" s="24"/>
-      <c r="I46" s="25"/>
-    </row>
-    <row r="47" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="33"/>
-      <c r="B47" s="5"/>
-      <c r="C47" s="10" t="s">
+      <c r="D47" s="4"/>
+      <c r="E47" s="4"/>
+      <c r="F47" s="21"/>
+      <c r="G47" s="21"/>
+      <c r="H47" s="21"/>
+      <c r="I47" s="21"/>
+    </row>
+    <row r="48" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="16"/>
+      <c r="B48" s="16"/>
+      <c r="C48" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D47" s="21"/>
-      <c r="E47" s="22"/>
-      <c r="F47" s="26"/>
-      <c r="G47" s="27"/>
-      <c r="H47" s="27"/>
-      <c r="I47" s="28"/>
-    </row>
-    <row r="48" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="33"/>
-      <c r="B48" s="5"/>
-      <c r="C48" s="10" t="s">
+      <c r="D48" s="4"/>
+      <c r="E48" s="4"/>
+      <c r="F48" s="21"/>
+      <c r="G48" s="21"/>
+      <c r="H48" s="21"/>
+      <c r="I48" s="21"/>
+    </row>
+    <row r="49" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="16"/>
+      <c r="B49" s="16"/>
+      <c r="C49" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="D48" s="21"/>
-      <c r="E48" s="22"/>
-      <c r="F48" s="23" t="s">
+      <c r="D49" s="4"/>
+      <c r="E49" s="5"/>
+      <c r="F49" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="G48" s="24"/>
-      <c r="H48" s="24"/>
-      <c r="I48" s="25"/>
-    </row>
-    <row r="49" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="34"/>
-      <c r="B49" s="35"/>
-      <c r="C49" s="10" t="s">
+      <c r="G49" s="7"/>
+      <c r="H49" s="7"/>
+      <c r="I49" s="8"/>
+    </row>
+    <row r="50" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="16"/>
+      <c r="B50" s="16"/>
+      <c r="C50" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D49" s="21"/>
-      <c r="E49" s="22"/>
-      <c r="F49" s="26"/>
-      <c r="G49" s="27"/>
-      <c r="H49" s="27"/>
-      <c r="I49" s="28"/>
-    </row>
-    <row r="50" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="D50" s="4"/>
+      <c r="E50" s="5"/>
+      <c r="F50" s="12"/>
+      <c r="G50" s="13"/>
+      <c r="H50" s="13"/>
+      <c r="I50" s="14"/>
+    </row>
     <row r="51" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="52" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="53" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="54" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="55" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="48">
-    <mergeCell ref="A43:B49"/>
-    <mergeCell ref="C45:E45"/>
-    <mergeCell ref="F43:I45"/>
-    <mergeCell ref="C43:E44"/>
+  <mergeCells count="49">
     <mergeCell ref="C46:E46"/>
-    <mergeCell ref="C47:E47"/>
-    <mergeCell ref="F46:I47"/>
-    <mergeCell ref="F48:I49"/>
-    <mergeCell ref="C48:E48"/>
-    <mergeCell ref="C49:E49"/>
-    <mergeCell ref="A1:I2"/>
-    <mergeCell ref="A3:B4"/>
-    <mergeCell ref="C7:E8"/>
-    <mergeCell ref="C5:E6"/>
-    <mergeCell ref="A5:B12"/>
-    <mergeCell ref="C3:E4"/>
-    <mergeCell ref="F3:I4"/>
+    <mergeCell ref="A43:B50"/>
+    <mergeCell ref="F46:I48"/>
+    <mergeCell ref="A13:B26"/>
+    <mergeCell ref="F34:I36"/>
+    <mergeCell ref="C34:E36"/>
+    <mergeCell ref="A27:B42"/>
+    <mergeCell ref="F27:I29"/>
+    <mergeCell ref="C37:E42"/>
+    <mergeCell ref="F37:I42"/>
+    <mergeCell ref="F30:I33"/>
+    <mergeCell ref="C32:E33"/>
+    <mergeCell ref="C21:E22"/>
+    <mergeCell ref="C23:E24"/>
+    <mergeCell ref="F21:I26"/>
+    <mergeCell ref="C30:E31"/>
+    <mergeCell ref="C27:E27"/>
+    <mergeCell ref="C28:E28"/>
     <mergeCell ref="C29:E29"/>
     <mergeCell ref="F17:I20"/>
     <mergeCell ref="F9:I12"/>
@@ -1471,21 +1478,21 @@
     <mergeCell ref="C19:E19"/>
     <mergeCell ref="C20:E20"/>
     <mergeCell ref="C25:E26"/>
-    <mergeCell ref="A13:B26"/>
-    <mergeCell ref="F34:I36"/>
-    <mergeCell ref="C34:E36"/>
-    <mergeCell ref="A27:B42"/>
-    <mergeCell ref="F27:I29"/>
-    <mergeCell ref="C37:E42"/>
-    <mergeCell ref="F37:I42"/>
-    <mergeCell ref="F30:I33"/>
-    <mergeCell ref="C32:E33"/>
-    <mergeCell ref="C21:E22"/>
-    <mergeCell ref="C23:E24"/>
-    <mergeCell ref="F21:I26"/>
-    <mergeCell ref="C30:E31"/>
-    <mergeCell ref="C27:E27"/>
-    <mergeCell ref="C28:E28"/>
+    <mergeCell ref="A1:I2"/>
+    <mergeCell ref="A3:B4"/>
+    <mergeCell ref="C7:E8"/>
+    <mergeCell ref="C5:E6"/>
+    <mergeCell ref="A5:B12"/>
+    <mergeCell ref="C3:E4"/>
+    <mergeCell ref="F3:I4"/>
+    <mergeCell ref="C45:E45"/>
+    <mergeCell ref="F43:I45"/>
+    <mergeCell ref="C43:E44"/>
+    <mergeCell ref="C47:E47"/>
+    <mergeCell ref="C48:E48"/>
+    <mergeCell ref="F49:I50"/>
+    <mergeCell ref="C49:E49"/>
+    <mergeCell ref="C50:E50"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>